<commit_message>
Changes for FedEx and H3P
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6480" uniqueCount="466">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="496">
   <si>
     <t>Service</t>
   </si>
@@ -1828,6 +1828,120 @@
 Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.199, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:55941}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
 Session ID: 272919927ff227e9c1f172d4db2bb85d
 *** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10218453</t>
+  </si>
+  <si>
+    <t>10218457</t>
+  </si>
+  <si>
+    <t>10218467</t>
+  </si>
+  <si>
+    <t>10218475</t>
+  </si>
+  <si>
+    <t>10218521</t>
+  </si>
+  <si>
+    <t>10218526</t>
+  </si>
+  <si>
+    <t>10218600</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=119.0.6045.199)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.26', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.199, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:56799}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: bea3aa9137144e3b64089285f98c5ec7
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10218606</t>
+  </si>
+  <si>
+    <t>136347778</t>
+  </si>
+  <si>
+    <t>10218820</t>
+  </si>
+  <si>
+    <t>10218826</t>
+  </si>
+  <si>
+    <t>10218840</t>
+  </si>
+  <si>
+    <t>10218844</t>
+  </si>
+  <si>
+    <t>10218858</t>
+  </si>
+  <si>
+    <t>10218868</t>
+  </si>
+  <si>
+    <t>10218879</t>
+  </si>
+  <si>
+    <t>10221568</t>
+  </si>
+  <si>
+    <t>10221569</t>
+  </si>
+  <si>
+    <t>10221579</t>
+  </si>
+  <si>
+    <t>10221599</t>
+  </si>
+  <si>
+    <t>10221605</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=119.0.6045.200)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.29', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.200, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53138}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: cac3fd6165c66cbed9d8cab7df90ac62
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10221617</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=119.0.6045.200)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.29', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.200, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58698}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 9e620668373f11d91f466650b7e55573
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10221733</t>
+  </si>
+  <si>
+    <t>10221741</t>
+  </si>
+  <si>
+    <t>10221744</t>
+  </si>
+  <si>
+    <t>10221749</t>
+  </si>
+  <si>
+    <t>136382364</t>
   </si>
 </sst>
 </file>
@@ -2262,7 +2376,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>458</v>
+        <v>483</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -2280,7 +2394,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>459</v>
+        <v>484</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -2298,14 +2412,14 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>460</v>
+        <v>485</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>79</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -2316,7 +2430,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>461</v>
+        <v>486</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -2424,14 +2538,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>462</v>
+        <v>491</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2442,14 +2556,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>463</v>
+        <v>492</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
+        <v>490</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2460,14 +2574,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>464</v>
+        <v>493</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>465</v>
+        <v>490</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2478,14 +2592,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>448</v>
+        <v>494</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>465</v>
+        <v>490</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2660,11 +2774,11 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>449</v>
+        <v>495</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F24" t="s">
         <v>147</v>
@@ -2682,7 +2796,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F25" t="s">
         <v>82</v>

</xml_diff>

<commit_message>
Changes of 5th Dec 2023
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6710" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6804" uniqueCount="509">
   <si>
     <t>Service</t>
   </si>
@@ -1942,6 +1942,61 @@
   </si>
   <si>
     <t>136382364</t>
+  </si>
+  <si>
+    <t>10223075</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=119.0.6045.200)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.14', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.200, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59709}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 79cab587ed4151dfc644fdef3c00d341
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10223102</t>
+  </si>
+  <si>
+    <t>10223105</t>
+  </si>
+  <si>
+    <t>10223119</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: headless chrome=119.0.6045.200)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.14', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 119.0.6045.200, chrome: {chromedriverVersion: 119.0.6045.105 (38c72552c5e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60496}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: b7e61e79fe2d4e962a4e6aeb1522a4a5
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10223226</t>
+  </si>
+  <si>
+    <t>10223231</t>
+  </si>
+  <si>
+    <t>10223233</t>
+  </si>
+  <si>
+    <t>10223246</t>
+  </si>
+  <si>
+    <t>10223256</t>
+  </si>
+  <si>
+    <t>136398862</t>
+  </si>
+  <si>
+    <t>10223388</t>
   </si>
 </sst>
 </file>
@@ -2376,7 +2431,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -2394,7 +2449,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>484</v>
+        <v>499</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -2412,7 +2467,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>485</v>
+        <v>508</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -2430,14 +2485,14 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>486</v>
+        <v>502</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
         <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -2538,14 +2593,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>491</v>
+        <v>503</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>501</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -2556,14 +2611,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>492</v>
+        <v>504</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -2574,14 +2629,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>493</v>
+        <v>505</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -2592,14 +2647,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>494</v>
+        <v>506</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>490</v>
+        <v>501</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2774,7 +2829,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>495</v>
+        <v>507</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">

</xml_diff>

<commit_message>
CHanges of order sequence
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7480" uniqueCount="614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7594" uniqueCount="633">
   <si>
     <t>Service</t>
   </si>
@@ -2434,6 +2434,71 @@
   </si>
   <si>
     <t>10233419</t>
+  </si>
+  <si>
+    <t>10234091</t>
+  </si>
+  <si>
+    <t>10234108</t>
+  </si>
+  <si>
+    <t>10234115</t>
+  </si>
+  <si>
+    <t>10234116</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.110)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.37', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.110, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62982}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 38ad931a7ef8dd60159bc4e7d91db684
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10234121</t>
+  </si>
+  <si>
+    <t>10234212</t>
+  </si>
+  <si>
+    <t>10234214</t>
+  </si>
+  <si>
+    <t>10234216</t>
+  </si>
+  <si>
+    <t>136532103</t>
+  </si>
+  <si>
+    <t>10234686</t>
+  </si>
+  <si>
+    <t>10234687</t>
+  </si>
+  <si>
+    <t>10234689</t>
+  </si>
+  <si>
+    <t>10234691</t>
+  </si>
+  <si>
+    <t>10234708</t>
+  </si>
+  <si>
+    <t>10234710</t>
+  </si>
+  <si>
+    <t>10234717</t>
+  </si>
+  <si>
+    <t>10234718</t>
+  </si>
+  <si>
+    <t>136546157</t>
   </si>
 </sst>
 </file>
@@ -2868,7 +2933,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>602</v>
+        <v>624</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -2886,7 +2951,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>603</v>
+        <v>625</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -2904,7 +2969,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>604</v>
+        <v>626</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -2922,7 +2987,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>605</v>
+        <v>627</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -3030,7 +3095,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>608</v>
+        <v>628</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -3048,14 +3113,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>609</v>
+        <v>629</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>607</v>
+        <v>618</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -3066,14 +3131,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>613</v>
+        <v>630</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>610</v>
+        <v>618</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -3084,14 +3149,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>611</v>
+        <v>631</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>607</v>
+        <v>618</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -3266,7 +3331,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>612</v>
+        <v>632</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">

</xml_diff>

<commit_message>
Final change for H3P
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7882" uniqueCount="682">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8112" uniqueCount="717">
   <si>
     <t>Service</t>
   </si>
@@ -2696,6 +2696,196 @@
   </si>
   <si>
     <t>10238914</t>
+  </si>
+  <si>
+    <t>10239783</t>
+  </si>
+  <si>
+    <t>10239785</t>
+  </si>
+  <si>
+    <t>10239790</t>
+  </si>
+  <si>
+    <t>10239791</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:65300}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: f63b34d008dae14134cd192282edbdc9
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239820</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63935}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a58470d7a423bab1eddb31856e0d89bd</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63935}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a58470d7a423bab1eddb31856e0d89bd
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239867</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:49529}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0680f7826512d94dd41832a7be1d1fa9
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239876</t>
+  </si>
+  <si>
+    <t>10239880</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58341}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 986b9e46a2932f32791e4c2ec1b9f8ac
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:54671}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: d79f71bc898b78325417aa5a24b63dc4
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239888</t>
+  </si>
+  <si>
+    <t>10239894</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:62098}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 9e30d83a180b136bd19acb95c6957101
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239904</t>
+  </si>
+  <si>
+    <t>10239910</t>
+  </si>
+  <si>
+    <t>10239913</t>
+  </si>
+  <si>
+    <t>10239920</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:51479}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 142b5189da12088a08eef83c19237bc7</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:51479}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 142b5189da12088a08eef83c19237bc7
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10239975</t>
+  </si>
+  <si>
+    <t>element not interactable: https://testdevna.nglog.com/TaskLog has no size and location
+  (Session info: chrome=120.0.6099.130)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60328}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 464a1670352f605194d2014e6b221a36</t>
+  </si>
+  <si>
+    <t>10239988</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome=120.0.6099.130)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.17', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58282}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: e92ca8ed5be11312d23177ae11763ce9
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10240140</t>
+  </si>
+  <si>
+    <t>10240182</t>
+  </si>
+  <si>
+    <t>10240197</t>
+  </si>
+  <si>
+    <t>10240204</t>
+  </si>
+  <si>
+    <t>10240218</t>
+  </si>
+  <si>
+    <t>136598488</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of [[ChromeDriver: chrome on WINDOWS (a877f57c0631f185a54ab0cbc4424a0d)] -&gt; id: GreyTick] (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.76', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 120.0.6099.130, chrome: {chromedriverVersion: 120.0.6099.109 (3419140ab66..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59665}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a877f57c0631f185a54ab0cbc4424a0d</t>
+  </si>
+  <si>
+    <t>10240223</t>
   </si>
 </sst>
 </file>
@@ -3130,14 +3320,14 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>674</v>
+        <v>696</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -3148,14 +3338,14 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>675</v>
+        <v>700</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -3166,7 +3356,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>676</v>
+        <v>701</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -3184,14 +3374,14 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>677</v>
+        <v>710</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
         <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -3292,14 +3482,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>681</v>
+        <v>716</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>56</v>
+        <v>704</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3310,14 +3500,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>678</v>
+        <v>711</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>673</v>
+        <v>708</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -3328,14 +3518,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>679</v>
+        <v>712</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>673</v>
+        <v>708</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -3346,14 +3536,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>680</v>
+        <v>713</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>673</v>
+        <v>708</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -3528,7 +3718,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>667</v>
+        <v>714</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -3571,7 +3761,7 @@
         <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>715</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>

</xml_diff>

<commit_message>
CHanges of 30th Jan
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8527" uniqueCount="791">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8594" uniqueCount="802">
   <si>
     <t>Service</t>
   </si>
@@ -3179,6 +3179,47 @@
   </si>
   <si>
     <t>136832320</t>
+  </si>
+  <si>
+    <t>10262084</t>
+  </si>
+  <si>
+    <t>10262092</t>
+  </si>
+  <si>
+    <t>10262104</t>
+  </si>
+  <si>
+    <t>10262110</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.85)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.69', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.85, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:64237}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: d4804c12644307a50394ee1d762ff46a
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10262150</t>
+  </si>
+  <si>
+    <t>10262154</t>
+  </si>
+  <si>
+    <t>10262208</t>
+  </si>
+  <si>
+    <t>10262211</t>
+  </si>
+  <si>
+    <t>10262213</t>
+  </si>
+  <si>
+    <t>136839363</t>
   </si>
 </sst>
 </file>
@@ -3613,7 +3654,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>778</v>
+        <v>791</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -3631,7 +3672,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>779</v>
+        <v>792</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -3649,7 +3690,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>786</v>
+        <v>793</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -3667,7 +3708,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>780</v>
+        <v>794</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -3775,14 +3816,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>789</v>
+        <v>800</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>785</v>
+        <v>795</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3793,14 +3834,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>787</v>
+        <v>798</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>733</v>
+        <v>795</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -3811,7 +3852,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>782</v>
+        <v>796</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
@@ -3829,14 +3870,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>788</v>
+        <v>799</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>784</v>
+        <v>56</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4011,7 +4052,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>790</v>
+        <v>801</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">

</xml_diff>

<commit_message>
Changes of wait issue on NA
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8635" uniqueCount="809">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8843" uniqueCount="840">
   <si>
     <t>Service</t>
   </si>
@@ -3241,6 +3241,175 @@
   </si>
   <si>
     <t>136895718</t>
+  </si>
+  <si>
+    <t>10267199</t>
+  </si>
+  <si>
+    <t>10267204</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.62', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58911}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 94d3d3ca37c466c895b4e2eb0f3e2d5b</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.62', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:58911}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 94d3d3ca37c466c895b4e2eb0f3e2d5b
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10267233</t>
+  </si>
+  <si>
+    <t>Cannot invoke "org.openqa.selenium.WebElement.clear()" because the return value of "connect_OCBaseMethods.OrderCreation.isElementPresent(String)" is null</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.62', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60460}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 04d45728d7764dee35627ccea70e7e3c
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of element located by By.id: hlkOrderSearch (tried for 50 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>10267271</t>
+  </si>
+  <si>
+    <t>10267278</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.47', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52762}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 808ea59d6c281e6d37651adf4fbb2f7b</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.47', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:52762}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 808ea59d6c281e6d37651adf4fbb2f7b
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10267285</t>
+  </si>
+  <si>
+    <t>10267286</t>
+  </si>
+  <si>
+    <t>10267296</t>
+  </si>
+  <si>
+    <t>10267302</t>
+  </si>
+  <si>
+    <t>10267311</t>
+  </si>
+  <si>
+    <t>10267312</t>
+  </si>
+  <si>
+    <t>136902504</t>
+  </si>
+  <si>
+    <t>10269059</t>
+  </si>
+  <si>
+    <t>10269064</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.60', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:59785}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 0ec92c51aa63d790c44806abf22c1644
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10269073</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.60', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:51600}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 42242f21495cfd6b75e8aa91fa4d96a0
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10269082</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.7', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60269}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 24216c9377acda6f570e24bc430c143e</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.7', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:60269}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 24216c9377acda6f570e24bc430c143e
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10269140</t>
+  </si>
+  <si>
+    <t>10269152</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.className: panel-body (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.7', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53882}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 86d56ff2c27acd402c43a7160cb35ffb</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.161)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.140.7', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '19.0.1'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.161, chrome: {chromedriverVersion: 121.0.6167.85 (3f98d690ad7e..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53882}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 86d56ff2c27acd402c43a7160cb35ffb
+*** Element info: {Using=id, value=lblServiceID}</t>
   </si>
 </sst>
 </file>
@@ -3675,14 +3844,14 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>791</v>
+        <v>831</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>50</v>
+        <v>832</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -3693,14 +3862,14 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>792</v>
+        <v>836</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>56</v>
+        <v>834</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -3711,14 +3880,14 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>793</v>
+        <v>837</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>838</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -3729,14 +3898,14 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>794</v>
+        <v>822</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G5" s="3"/>
       <c r="H5" s="3"/>
@@ -3837,14 +4006,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>807</v>
+        <v>826</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F11" t="s">
-        <v>795</v>
+        <v>839</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -3855,14 +4024,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>802</v>
+        <v>823</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>795</v>
+        <v>839</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -3873,14 +4042,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>803</v>
+        <v>824</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
-        <v>733</v>
+        <v>839</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -3891,14 +4060,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>804</v>
+        <v>825</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F14" t="s">
-        <v>56</v>
+        <v>839</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4060,7 +4229,7 @@
         <v>51</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
+        <v>814</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3"/>
@@ -4073,11 +4242,11 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>808</v>
+        <v>827</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F24" t="s">
         <v>147</v>
@@ -4095,7 +4264,7 @@
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="F25" t="s">
         <v>82</v>
@@ -4116,7 +4285,7 @@
         <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>

</xml_diff>

<commit_message>
Changes of 26th Feb 2024
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9068" uniqueCount="875">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9150" uniqueCount="886">
   <si>
     <t>Service</t>
   </si>
@@ -3536,6 +3536,47 @@
   </si>
   <si>
     <t>136984827</t>
+  </si>
+  <si>
+    <t>10275953</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=121.0.6167.189)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.41', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 121.0.6167.189, chrome: {chromedriverVersion: 121.0.6167.184 (057a8ae7deb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:50375}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 4e0b85e0b26caa43044a6b7ed4319fa7
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>10276024</t>
+  </si>
+  <si>
+    <t>10276026</t>
+  </si>
+  <si>
+    <t>10276032</t>
+  </si>
+  <si>
+    <t>10276039</t>
+  </si>
+  <si>
+    <t>10276068</t>
+  </si>
+  <si>
+    <t>10276077</t>
+  </si>
+  <si>
+    <t>10276082</t>
+  </si>
+  <si>
+    <t>10276088</t>
+  </si>
+  <si>
+    <t>137010051</t>
   </si>
 </sst>
 </file>
@@ -3970,14 +4011,14 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>866</v>
+        <v>877</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>832</v>
+        <v>56</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -3988,14 +4029,14 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>867</v>
+        <v>878</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>834</v>
+        <v>52</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -4006,7 +4047,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>868</v>
+        <v>879</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -4024,7 +4065,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>869</v>
+        <v>880</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -4132,14 +4173,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>873</v>
+        <v>884</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -4150,14 +4191,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>870</v>
+        <v>881</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -4168,14 +4209,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>871</v>
+        <v>882</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -4186,14 +4227,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>872</v>
+        <v>883</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>853</v>
+        <v>876</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4368,7 +4409,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>874</v>
+        <v>885</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">

</xml_diff>

<commit_message>
Changes of prod Uname pwd
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9150" uniqueCount="886">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9295" uniqueCount="909">
   <si>
     <t>Service</t>
   </si>
@@ -3577,6 +3577,75 @@
   </si>
   <si>
     <t>137010051</t>
+  </si>
+  <si>
+    <t>10284452</t>
+  </si>
+  <si>
+    <t>10284463</t>
+  </si>
+  <si>
+    <t>10284473</t>
+  </si>
+  <si>
+    <t>10284488</t>
+  </si>
+  <si>
+    <t>10284531</t>
+  </si>
+  <si>
+    <t>10284549</t>
+  </si>
+  <si>
+    <t>10284562</t>
+  </si>
+  <si>
+    <t>10284565</t>
+  </si>
+  <si>
+    <t>137103548</t>
+  </si>
+  <si>
+    <t>10290936</t>
+  </si>
+  <si>
+    <t>10290952</t>
+  </si>
+  <si>
+    <t>10290995</t>
+  </si>
+  <si>
+    <t>10291051</t>
+  </si>
+  <si>
+    <t>10291068</t>
+  </si>
+  <si>
+    <t>10293410</t>
+  </si>
+  <si>
+    <t>10293415</t>
+  </si>
+  <si>
+    <t>10293432</t>
+  </si>
+  <si>
+    <t>10293446</t>
+  </si>
+  <si>
+    <t>10293457</t>
+  </si>
+  <si>
+    <t>10293466</t>
+  </si>
+  <si>
+    <t>10293476</t>
+  </si>
+  <si>
+    <t>10293483</t>
+  </si>
+  <si>
+    <t>137200001</t>
   </si>
 </sst>
 </file>
@@ -4011,7 +4080,7 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>877</v>
+        <v>900</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
@@ -4029,14 +4098,14 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>878</v>
+        <v>901</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
         <v>51</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G3" s="3"/>
       <c r="H3" s="3"/>
@@ -4047,7 +4116,7 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>879</v>
+        <v>902</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
@@ -4065,7 +4134,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>880</v>
+        <v>903</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -4173,7 +4242,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>884</v>
+        <v>907</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
@@ -4191,7 +4260,7 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>881</v>
+        <v>904</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
@@ -4209,7 +4278,7 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>882</v>
+        <v>905</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
@@ -4227,7 +4296,7 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>883</v>
+        <v>906</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
@@ -4409,7 +4478,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>885</v>
+        <v>908</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">

</xml_diff>

<commit_message>
Changes of Operations label renamed by Shipments label
</commit_message>
<xml_diff>
--- a/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
+++ b/NetAgent/src/main/resources/NA OCP Result_Test.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9364" uniqueCount="923">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9497" uniqueCount="942">
   <si>
     <t>Service</t>
   </si>
@@ -3693,6 +3693,94 @@
   </si>
   <si>
     <t>10294944</t>
+  </si>
+  <si>
+    <t>10295959</t>
+  </si>
+  <si>
+    <t>10295966</t>
+  </si>
+  <si>
+    <t>10299995</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of element located by By.id: lblServiceID (tried for 30 second(s) with 500 milliseconds interval)</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=122.0.6261.129)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.43', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a15c90a65f3c3f855ff37c45702fa158
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.id: AdvancesSearch (tried for 50 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.43', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:53370}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: a15c90a65f3c3f855ff37c45702fa158</t>
+  </si>
+  <si>
+    <t>10300009</t>
+  </si>
+  <si>
+    <t>10300015</t>
+  </si>
+  <si>
+    <t>10300024</t>
+  </si>
+  <si>
+    <t>no such element: Unable to locate element: {"method":"css selector","selector":"#lblServiceID"}
+  (Session info: chrome-headless-shell=122.0.6261.129)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/no_such_element.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.16', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome-headless-shell, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:63458}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 3e8e4ea869dab0400e39a0f5e6cf0ea0
+*** Element info: {Using=id, value=lblServiceID}</t>
+  </si>
+  <si>
+    <t>137274899</t>
+  </si>
+  <si>
+    <t>10300116</t>
+  </si>
+  <si>
+    <t>10300117</t>
+  </si>
+  <si>
+    <t>10300121</t>
+  </si>
+  <si>
+    <t>10300129</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for visibility of all elements located by By.xpath: //*[@ng-form="FDXUPSFOrm"] (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:49604}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 90906add1415bc7936b4e50a6a63f496</t>
+  </si>
+  <si>
+    <t>10300177</t>
+  </si>
+  <si>
+    <t>Expected condition failed: waiting for element to be clickable: [[ChromeDriver: chrome on WINDOWS (90906add1415bc7936b4e50a6a63f496)] -&gt; xpath: //a[@id="idTask"]] (tried for 60 second(s) with 500 milliseconds interval)
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'SIPL92', ip: '10.212.130.2', os.name: 'Windows 10', os.arch: 'amd64', os.version: '10.0', java.version: '20'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 122.0.6261.129, chrome: {chromedriverVersion: 122.0.6261.128 (f18a44fedeb..., userDataDir: C:\Users\RPRAJA~1\AppData\L...}, fedcm:accounts: true, goog:chromeOptions: {debuggerAddress: localhost:49604}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: WINDOWS, platformName: WINDOWS, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:credBlob: true, webauthn:extension:largeBlob: true, webauthn:extension:minPinLength: true, webauthn:extension:prf: true, webauthn:virtualAuthenticators: true}
+Session ID: 90906add1415bc7936b4e50a6a63f496</t>
+  </si>
+  <si>
+    <t>10300215</t>
   </si>
 </sst>
 </file>
@@ -4127,14 +4215,14 @@
       </c>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
-        <v>921</v>
+        <v>929</v>
       </c>
       <c r="D2" s="1"/>
       <c r="E2" t="s">
         <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>926</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
@@ -4145,7 +4233,7 @@
       </c>
       <c r="B3" s="1"/>
       <c r="C3" t="s">
-        <v>922</v>
+        <v>930</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" t="s">
@@ -4163,14 +4251,14 @@
       </c>
       <c r="B4" s="1"/>
       <c r="C4" t="s">
-        <v>913</v>
+        <v>941</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" t="s">
         <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>940</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="3"/>
@@ -4181,7 +4269,7 @@
       </c>
       <c r="B5" s="1"/>
       <c r="C5" t="s">
-        <v>914</v>
+        <v>931</v>
       </c>
       <c r="D5" s="1"/>
       <c r="E5" t="s">
@@ -4289,14 +4377,14 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" t="s">
-        <v>918</v>
+        <v>937</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" t="s">
         <v>51</v>
       </c>
       <c r="F11" t="s">
-        <v>876</v>
+        <v>932</v>
       </c>
       <c r="G11" s="3"/>
       <c r="H11" s="3"/>
@@ -4307,14 +4395,14 @@
       </c>
       <c r="B12" s="1"/>
       <c r="C12" t="s">
-        <v>915</v>
+        <v>934</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
         <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>876</v>
+        <v>932</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -4325,14 +4413,14 @@
       </c>
       <c r="B13" s="1"/>
       <c r="C13" t="s">
-        <v>916</v>
+        <v>935</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
         <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>876</v>
+        <v>932</v>
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
@@ -4343,14 +4431,14 @@
       </c>
       <c r="B14" s="1"/>
       <c r="C14" t="s">
-        <v>917</v>
+        <v>936</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
         <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>876</v>
+        <v>932</v>
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -4404,7 +4492,7 @@
         <v>51</v>
       </c>
       <c r="F17" t="s">
-        <v>56</v>
+        <v>361</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3"/>
@@ -4419,10 +4507,10 @@
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F18" t="s">
-        <v>56</v>
+        <v>938</v>
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3"/>
@@ -4525,7 +4613,7 @@
         <v>32</v>
       </c>
       <c r="C24" t="s">
-        <v>919</v>
+        <v>933</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" t="s">
@@ -4568,7 +4656,7 @@
         <v>49</v>
       </c>
       <c r="F26" t="s">
-        <v>920</v>
+        <v>56</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>

</xml_diff>